<commit_message>
User stories med prioriteringer
</commit_message>
<xml_diff>
--- a/doc/ITimeU_User_stories_estimated.xlsx
+++ b/doc/ITimeU_User_stories_estimated.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>User story</t>
   </si>
@@ -150,25 +150,37 @@
     <t>As a spectator I want to see the result in real time so that I can follow the event live.</t>
   </si>
   <si>
-    <t>Buiness value</t>
-  </si>
-  <si>
     <t>ROI</t>
   </si>
   <si>
-    <t>As an administrator I want to be notified if something is going wroing during import so that I know what data did'nt get imported</t>
-  </si>
-  <si>
     <t>As a time keeper I want the time automatically saved during a race so I don't have to do it manually</t>
   </si>
   <si>
-    <t>As an administrator I want to be able to edit the resultlist so that any changes can be made</t>
-  </si>
-  <si>
     <t>As an administrator I want to merge the time results and the order of the starting number at the finish, so I get a merged list with finishing time and the corresponding correct starting number</t>
   </si>
   <si>
-    <t>User stories not estimated (but still very important requirement the system must fulfill)</t>
+    <t>ITimeU User Stories</t>
+  </si>
+  <si>
+    <t>Business value</t>
+  </si>
+  <si>
+    <t>As an administrator I want to be notified if something is going wrong during import so that I know what data didn't get imported</t>
+  </si>
+  <si>
+    <t>As an administrator I want to be able to edit the result list so that any changes can be made</t>
+  </si>
+  <si>
+    <t>User stories not estimated (but still very important fundamental requirement the system must fulfil)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Not relevant since the system is going to be offline.</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -176,9 +188,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +241,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -315,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -350,15 +369,26 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -666,17 +696,20 @@
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -684,411 +717,559 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F3" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11">
+        <f>C4/B4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" ht="27.75" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:D39" si="0">C5/B5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" ht="27.75" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="27.75" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7">
         <v>3</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C9" s="10"/>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C10" s="10"/>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" ht="27.75" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="41.25" thickBot="1">
+      <c r="C11" s="10"/>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="41.25" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C12" s="10"/>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="27.75" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" ht="41.25" thickBot="1">
-      <c r="A14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C13" s="10"/>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="41.25" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="27.75" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="7">
         <v>2</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C15" s="10"/>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" ht="27.75" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="7">
         <v>2</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C16" s="10"/>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" ht="27.75" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7">
         <v>3</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C17" s="10"/>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" ht="27.75" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7">
         <v>2</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C18" s="10"/>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="27.75" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C19" s="10"/>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="7">
         <v>13</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C20" s="10"/>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="7">
         <v>8</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A22" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C21" s="10"/>
+      <c r="D21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="27.75" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="7">
         <v>8</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C23" s="10"/>
+      <c r="D23" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="27.75" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C24" s="10"/>
+      <c r="D24" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" ht="27.75" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="7">
         <v>5</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C25" s="10"/>
+      <c r="D25" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" ht="27.75" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="7">
         <v>3</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C26" s="10"/>
+      <c r="D26" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="27.75" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="7">
         <v>3</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="27.75" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7">
         <v>2</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" ht="41.25" thickBot="1">
+      <c r="C28" s="10"/>
+      <c r="D28" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="41.25" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="7">
         <v>3</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C29" s="10"/>
+      <c r="D29" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" ht="27.75" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="7">
         <v>2</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:4" ht="41.25" thickBot="1">
+      <c r="C30" s="10"/>
+      <c r="D30" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A31" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" ht="41.25" thickBot="1">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="7">
-        <v>3</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B32" s="7"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="7"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" ht="27.75" thickBot="1">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:4" ht="27.75" thickBot="1">
+      <c r="C34" s="10"/>
+      <c r="D34" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" ht="27.75" thickBot="1">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="7">
         <v>2</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A36" s="5" t="s">
+      <c r="C35" s="10"/>
+      <c r="D35" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A37" s="5" t="s">
+      <c r="C37" s="10"/>
+      <c r="D37" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B38" s="7">
         <v>2</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A38" s="5" t="s">
+      <c r="C38" s="10"/>
+      <c r="D38" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B39" s="7">
         <v>3</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:4" ht="41.25" thickBot="1">
-      <c r="A39" s="6" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="1:6" ht="41.25" thickBot="1">
+      <c r="A40" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A40" s="6" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="F40" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A41" s="6" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="F41" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A42" s="6" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="F42" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A46" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="27.75" thickBot="1">
-      <c r="A47" s="9" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="F43" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A47" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="27.75" thickBot="1">
+      <c r="A48" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="41.25" thickBot="1">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:1" ht="41.25" thickBot="1">
+      <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="27.75" thickBot="1">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:1" ht="27.75" thickBot="1">
+      <c r="A50" s="5" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
User storiesn naa med prioriteringer
</commit_message>
<xml_diff>
--- a/doc/ITimeU_User_stories_estimated.xlsx
+++ b/doc/ITimeU_User_stories_estimated.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>User story</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Could be checked manually I guess</t>
+  </si>
+  <si>
+    <t>This should normally be part of the import, yes</t>
+  </si>
+  <si>
+    <t>A warning is enough</t>
   </si>
 </sst>
 </file>
@@ -687,7 +696,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,10 +742,12 @@
       <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="10">
+        <v>5</v>
+      </c>
       <c r="D4" s="11">
         <f>C4/B4</f>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F4" s="14"/>
     </row>
@@ -747,10 +758,12 @@
       <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="10">
+        <v>5</v>
+      </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5:D39" si="0">C5/B5</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F5" s="14"/>
     </row>
@@ -761,10 +774,12 @@
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10">
+        <v>3</v>
+      </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="14"/>
     </row>
@@ -775,10 +790,12 @@
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -787,7 +804,9 @@
         <v>41</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10">
+        <v>2</v>
+      </c>
       <c r="D8" s="11"/>
       <c r="F8" s="14"/>
     </row>
@@ -798,10 +817,12 @@
       <c r="B9" s="7">
         <v>3</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10">
+        <v>4</v>
+      </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F9" s="14"/>
     </row>
@@ -812,10 +833,12 @@
       <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10">
+        <v>5</v>
+      </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="14"/>
     </row>
@@ -826,10 +849,12 @@
       <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10">
+        <v>5</v>
+      </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F11" s="14"/>
     </row>
@@ -840,10 +865,12 @@
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F12" s="14"/>
     </row>
@@ -854,10 +881,12 @@
       <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="10">
+        <v>5</v>
+      </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F13" s="14"/>
     </row>
@@ -866,7 +895,9 @@
         <v>42</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="10">
+        <v>5</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="F14" s="14"/>
     </row>
@@ -877,10 +908,12 @@
       <c r="B15" s="7">
         <v>2</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="10">
+        <v>3</v>
+      </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F15" s="14"/>
     </row>
@@ -891,10 +924,12 @@
       <c r="B16" s="7">
         <v>2</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="10">
+        <v>5</v>
+      </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F16" s="14"/>
     </row>
@@ -905,10 +940,12 @@
       <c r="B17" s="7">
         <v>3</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10">
+        <v>4</v>
+      </c>
       <c r="D17" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F17" s="14"/>
     </row>
@@ -919,10 +956,12 @@
       <c r="B18" s="7">
         <v>2</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="10">
+        <v>4</v>
+      </c>
       <c r="D18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="14"/>
     </row>
@@ -933,10 +972,12 @@
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="10">
+        <v>5</v>
+      </c>
       <c r="D19" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F19" s="14"/>
     </row>
@@ -947,10 +988,12 @@
       <c r="B20" s="7">
         <v>13</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="10">
+        <v>4</v>
+      </c>
       <c r="D20" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="F20" s="14"/>
     </row>
@@ -961,10 +1004,12 @@
       <c r="B21" s="7">
         <v>8</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
       <c r="D21" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="F21" s="14"/>
     </row>
@@ -973,8 +1018,13 @@
         <v>45</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10">
+        <v>2</v>
+      </c>
       <c r="D22" s="11"/>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="27.75" thickBot="1">
@@ -984,10 +1034,15 @@
       <c r="B23" s="7">
         <v>8</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
       <c r="D23" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.375</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
       </c>
       <c r="F23" s="14"/>
     </row>
@@ -998,10 +1053,12 @@
       <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="10">
+        <v>5</v>
+      </c>
       <c r="D24" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F24" s="14"/>
     </row>
@@ -1012,10 +1069,12 @@
       <c r="B25" s="7">
         <v>5</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="10">
+        <v>5</v>
+      </c>
       <c r="D25" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="14"/>
     </row>
@@ -1026,10 +1085,12 @@
       <c r="B26" s="7">
         <v>3</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="10">
+        <v>3</v>
+      </c>
       <c r="D26" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="14"/>
     </row>
@@ -1040,10 +1101,12 @@
       <c r="B27" s="7">
         <v>3</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="10">
+        <v>3</v>
+      </c>
       <c r="D27" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="14"/>
     </row>
@@ -1054,10 +1117,12 @@
       <c r="B28" s="7">
         <v>2</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="10">
+        <v>3</v>
+      </c>
       <c r="D28" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F28" s="14"/>
     </row>
@@ -1068,10 +1133,12 @@
       <c r="B29" s="7">
         <v>3</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="10">
+        <v>4</v>
+      </c>
       <c r="D29" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="F29" s="14"/>
     </row>
@@ -1082,10 +1149,15 @@
       <c r="B30" s="7">
         <v>2</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="10">
+        <v>1</v>
+      </c>
       <c r="D30" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
       </c>
       <c r="F30" s="14"/>
     </row>
@@ -1096,10 +1168,12 @@
       <c r="B31" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="10">
+        <v>5</v>
+      </c>
       <c r="D31" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="14"/>
     </row>
@@ -1108,7 +1182,9 @@
         <v>29</v>
       </c>
       <c r="B32" s="7"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="10">
+        <v>1</v>
+      </c>
       <c r="D32" s="11"/>
       <c r="F32" s="14"/>
     </row>
@@ -1128,10 +1204,12 @@
       <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="10">
+        <v>2</v>
+      </c>
       <c r="D34" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="14"/>
     </row>
@@ -1142,10 +1220,12 @@
       <c r="B35" s="7">
         <v>2</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="10">
+        <v>1</v>
+      </c>
       <c r="D35" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F35" s="14"/>
     </row>
@@ -1163,10 +1243,12 @@
       <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="10">
+        <v>3</v>
+      </c>
       <c r="D37" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="14"/>
     </row>
@@ -1177,10 +1259,12 @@
       <c r="B38" s="7">
         <v>2</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="10">
+        <v>2</v>
+      </c>
       <c r="D38" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="14"/>
     </row>
@@ -1191,10 +1275,12 @@
       <c r="B39" s="7">
         <v>3</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="10">
+        <v>5</v>
+      </c>
       <c r="D39" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F39" s="14"/>
     </row>
@@ -1256,15 +1342,24 @@
       <c r="A48" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="41.25" thickBot="1">
+      <c r="C48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="41.25" thickBot="1">
       <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="27.75" thickBot="1">
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="27.75" thickBot="1">
       <c r="A50" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>